<commit_message>
Now I'm stuck and it's broken
</commit_message>
<xml_diff>
--- a/docs/manualTesting/SDXL_Fantasy_TestMatrix.xlsx
+++ b/docs/manualTesting/SDXL_Fantasy_TestMatrix.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\projects\StableNew\docs\manualTesting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2A1F3-2069-4985-AB97-6D1431BE15F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4500" yWindow="5580" windowWidth="28950" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -100,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +170,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +222,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -242,6 +256,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,9 +291,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,14 +467,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -521,8 +549,23 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -539,7 +582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -556,7 +599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -573,7 +616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -590,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -607,7 +650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -624,7 +667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -640,8 +683,23 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -658,7 +716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -675,7 +733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -692,7 +750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -709,7 +767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -726,7 +784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -743,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -759,8 +817,23 @@
       <c r="E16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -777,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -794,7 +867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -811,7 +884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -828,7 +901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -845,7 +918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -862,7 +935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -878,8 +951,23 @@
       <c r="E23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -896,7 +984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -913,7 +1001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -930,7 +1018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -947,7 +1035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -964,7 +1052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>

</xml_diff>